<commit_message>
Ajout de la validation des numéros de téléphone
</commit_message>
<xml_diff>
--- a/vue-back-server/temp/erreurs_resume_latest.xlsx
+++ b/vue-back-server/temp/erreurs_resume_latest.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>544</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>